<commit_message>
updated app.js to remove main domain bootstrap from cart page
</commit_message>
<xml_diff>
--- a/URLRedirects.xlsx
+++ b/URLRedirects.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -180,9 +180,6 @@
     <t>/browse.cfm/4,3.html</t>
   </si>
   <si>
-    <t>2 turtle</t>
-  </si>
-  <si>
     <t>/browse.cfm/4,110.html</t>
   </si>
   <si>
@@ -1015,6 +1012,9 @@
   </si>
   <si>
     <t>6x6 winteberry pinecone</t>
+  </si>
+  <si>
+    <t>2 turtle doves orn</t>
   </si>
 </sst>
 </file>
@@ -1433,8 +1433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
-      <selection activeCell="A177" sqref="A177"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1677,10 +1677,10 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" t="s">
         <v>70</v>
-      </c>
-      <c r="B30" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -1688,108 +1688,108 @@
         <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>331</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" t="s">
         <v>54</v>
-      </c>
-      <c r="C32" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" t="s">
         <v>56</v>
-      </c>
-      <c r="C33" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" t="s">
         <v>58</v>
-      </c>
-      <c r="C34" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" t="s">
         <v>60</v>
-      </c>
-      <c r="C35" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C36" t="s">
         <v>62</v>
-      </c>
-      <c r="C36" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" t="s">
         <v>64</v>
-      </c>
-      <c r="C37" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" t="s">
         <v>66</v>
-      </c>
-      <c r="C38" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" t="s">
         <v>68</v>
-      </c>
-      <c r="C39" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" t="s">
         <v>75</v>
-      </c>
-      <c r="B41" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" t="s">
         <v>77</v>
-      </c>
-      <c r="C42" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
+        <v>78</v>
+      </c>
+      <c r="C43" t="s">
         <v>79</v>
-      </c>
-      <c r="C43" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B44" t="s">
         <v>4</v>
@@ -1797,26 +1797,26 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" t="s">
         <v>82</v>
-      </c>
-      <c r="C45" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" t="s">
         <v>84</v>
-      </c>
-      <c r="C46" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" t="s">
         <v>86</v>
-      </c>
-      <c r="C47" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1829,23 +1829,23 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
+        <v>87</v>
+      </c>
+      <c r="C49" t="s">
         <v>88</v>
-      </c>
-      <c r="C49" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
+        <v>89</v>
+      </c>
+      <c r="C50" t="s">
         <v>90</v>
-      </c>
-      <c r="C50" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B51" t="s">
         <v>9</v>
@@ -1853,47 +1853,47 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" t="s">
         <v>93</v>
-      </c>
-      <c r="C52" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" t="s">
         <v>95</v>
-      </c>
-      <c r="C53" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
+        <v>96</v>
+      </c>
+      <c r="C54" t="s">
         <v>97</v>
-      </c>
-      <c r="C54" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
+        <v>98</v>
+      </c>
+      <c r="C55" t="s">
         <v>99</v>
-      </c>
-      <c r="C55" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
+        <v>100</v>
+      </c>
+      <c r="C56" t="s">
         <v>101</v>
-      </c>
-      <c r="C56" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B57" t="s">
         <v>9</v>
@@ -1901,439 +1901,439 @@
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58" t="s">
         <v>104</v>
-      </c>
-      <c r="C58" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
+        <v>105</v>
+      </c>
+      <c r="C59" t="s">
         <v>106</v>
-      </c>
-      <c r="C59" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" t="s">
         <v>108</v>
-      </c>
-      <c r="C60" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
+        <v>109</v>
+      </c>
+      <c r="C61" t="s">
         <v>110</v>
-      </c>
-      <c r="C61" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
+        <v>111</v>
+      </c>
+      <c r="C62" t="s">
         <v>112</v>
-      </c>
-      <c r="C62" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
+        <v>113</v>
+      </c>
+      <c r="C63" t="s">
         <v>114</v>
-      </c>
-      <c r="C63" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
+        <v>115</v>
+      </c>
+      <c r="C64" t="s">
         <v>116</v>
-      </c>
-      <c r="C64" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
+        <v>117</v>
+      </c>
+      <c r="C65" t="s">
         <v>118</v>
-      </c>
-      <c r="C65" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
+        <v>119</v>
+      </c>
+      <c r="C66" t="s">
         <v>120</v>
-      </c>
-      <c r="C66" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
+        <v>121</v>
+      </c>
+      <c r="C67" t="s">
         <v>122</v>
-      </c>
-      <c r="C67" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
+        <v>123</v>
+      </c>
+      <c r="C68" t="s">
         <v>124</v>
-      </c>
-      <c r="C68" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
+        <v>125</v>
+      </c>
+      <c r="C69" t="s">
         <v>126</v>
-      </c>
-      <c r="C69" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
+        <v>127</v>
+      </c>
+      <c r="C70" t="s">
         <v>128</v>
-      </c>
-      <c r="C70" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
+        <v>129</v>
+      </c>
+      <c r="C71" t="s">
         <v>130</v>
-      </c>
-      <c r="C71" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
+        <v>131</v>
+      </c>
+      <c r="C72" t="s">
         <v>132</v>
-      </c>
-      <c r="C72" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
+        <v>133</v>
+      </c>
+      <c r="C73" t="s">
         <v>134</v>
-      </c>
-      <c r="C73" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
+        <v>135</v>
+      </c>
+      <c r="C74" t="s">
         <v>136</v>
-      </c>
-      <c r="C74" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
+        <v>137</v>
+      </c>
+      <c r="C75" t="s">
         <v>138</v>
-      </c>
-      <c r="C75" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
+        <v>139</v>
+      </c>
+      <c r="C76" t="s">
         <v>140</v>
-      </c>
-      <c r="C76" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
+        <v>141</v>
+      </c>
+      <c r="C77" t="s">
         <v>142</v>
-      </c>
-      <c r="C77" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
+        <v>143</v>
+      </c>
+      <c r="C78" t="s">
         <v>144</v>
-      </c>
-      <c r="C78" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
+        <v>145</v>
+      </c>
+      <c r="C79" t="s">
         <v>146</v>
-      </c>
-      <c r="C79" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C80" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
+        <v>148</v>
+      </c>
+      <c r="C81" t="s">
         <v>149</v>
-      </c>
-      <c r="C81" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
+        <v>150</v>
+      </c>
+      <c r="C82" t="s">
         <v>151</v>
-      </c>
-      <c r="C82" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
+        <v>152</v>
+      </c>
+      <c r="C83" t="s">
         <v>153</v>
-      </c>
-      <c r="C83" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
+        <v>154</v>
+      </c>
+      <c r="C84" t="s">
         <v>155</v>
-      </c>
-      <c r="C84" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
+        <v>156</v>
+      </c>
+      <c r="C85" t="s">
         <v>157</v>
-      </c>
-      <c r="C85" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
+        <v>158</v>
+      </c>
+      <c r="C86" t="s">
         <v>159</v>
-      </c>
-      <c r="C86" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
+        <v>160</v>
+      </c>
+      <c r="C87" t="s">
         <v>161</v>
-      </c>
-      <c r="C87" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
+        <v>162</v>
+      </c>
+      <c r="C88" t="s">
         <v>163</v>
-      </c>
-      <c r="C88" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
+        <v>164</v>
+      </c>
+      <c r="C89" t="s">
         <v>165</v>
-      </c>
-      <c r="C89" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
+        <v>166</v>
+      </c>
+      <c r="C90" t="s">
         <v>167</v>
-      </c>
-      <c r="C90" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
+        <v>168</v>
+      </c>
+      <c r="C91" t="s">
         <v>169</v>
-      </c>
-      <c r="C91" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
+        <v>170</v>
+      </c>
+      <c r="C92" t="s">
         <v>171</v>
-      </c>
-      <c r="C92" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
+        <v>172</v>
+      </c>
+      <c r="C93" t="s">
         <v>173</v>
-      </c>
-      <c r="C93" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
+        <v>174</v>
+      </c>
+      <c r="C94" t="s">
         <v>175</v>
-      </c>
-      <c r="C94" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C95" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
+        <v>177</v>
+      </c>
+      <c r="C96" t="s">
         <v>178</v>
-      </c>
-      <c r="C96" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
+        <v>179</v>
+      </c>
+      <c r="C97" t="s">
         <v>180</v>
-      </c>
-      <c r="C97" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
+        <v>181</v>
+      </c>
+      <c r="C98" t="s">
         <v>182</v>
-      </c>
-      <c r="C98" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
+        <v>183</v>
+      </c>
+      <c r="C99" t="s">
         <v>184</v>
-      </c>
-      <c r="C99" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
+        <v>185</v>
+      </c>
+      <c r="C100" t="s">
         <v>186</v>
-      </c>
-      <c r="C100" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
+        <v>187</v>
+      </c>
+      <c r="C101" t="s">
         <v>188</v>
-      </c>
-      <c r="C101" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
+        <v>189</v>
+      </c>
+      <c r="C102" t="s">
         <v>190</v>
-      </c>
-      <c r="C102" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
+        <v>191</v>
+      </c>
+      <c r="C103" t="s">
         <v>192</v>
-      </c>
-      <c r="C103" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
+        <v>193</v>
+      </c>
+      <c r="C104" t="s">
         <v>194</v>
-      </c>
-      <c r="C104" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
+        <v>195</v>
+      </c>
+      <c r="C105" t="s">
         <v>196</v>
-      </c>
-      <c r="C105" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
+        <v>197</v>
+      </c>
+      <c r="C106" t="s">
         <v>198</v>
-      </c>
-      <c r="C106" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
+        <v>199</v>
+      </c>
+      <c r="C107" t="s">
         <v>200</v>
-      </c>
-      <c r="C107" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
+        <v>201</v>
+      </c>
+      <c r="C108" t="s">
         <v>202</v>
-      </c>
-      <c r="C108" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
+        <v>203</v>
+      </c>
+      <c r="C109" t="s">
         <v>204</v>
-      </c>
-      <c r="C109" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
+        <v>205</v>
+      </c>
+      <c r="C110" t="s">
         <v>206</v>
-      </c>
-      <c r="C110" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
+        <v>207</v>
+      </c>
+      <c r="C111" t="s">
         <v>208</v>
-      </c>
-      <c r="C111" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B112" t="s">
         <v>9</v>
@@ -2341,95 +2341,95 @@
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
+        <v>210</v>
+      </c>
+      <c r="C113" t="s">
         <v>211</v>
-      </c>
-      <c r="C113" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
+        <v>212</v>
+      </c>
+      <c r="C114" t="s">
         <v>213</v>
-      </c>
-      <c r="C114" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
+        <v>214</v>
+      </c>
+      <c r="C115" t="s">
         <v>215</v>
-      </c>
-      <c r="C115" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
+        <v>216</v>
+      </c>
+      <c r="C116" t="s">
         <v>217</v>
-      </c>
-      <c r="C116" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
+        <v>218</v>
+      </c>
+      <c r="C117" t="s">
         <v>219</v>
-      </c>
-      <c r="C117" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
+        <v>220</v>
+      </c>
+      <c r="C118" t="s">
         <v>221</v>
-      </c>
-      <c r="C118" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
+        <v>222</v>
+      </c>
+      <c r="C119" t="s">
         <v>223</v>
-      </c>
-      <c r="C119" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
+        <v>224</v>
+      </c>
+      <c r="B120" t="s">
         <v>225</v>
-      </c>
-      <c r="B120" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
+        <v>226</v>
+      </c>
+      <c r="C121" t="s">
         <v>227</v>
-      </c>
-      <c r="C121" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
+        <v>228</v>
+      </c>
+      <c r="C122" t="s">
         <v>229</v>
-      </c>
-      <c r="C122" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
+        <v>230</v>
+      </c>
+      <c r="C123" t="s">
         <v>231</v>
-      </c>
-      <c r="C123" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B124" t="s">
         <v>9</v>
@@ -2437,7 +2437,7 @@
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B125" t="s">
         <v>9</v>
@@ -2445,410 +2445,410 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
+        <v>234</v>
+      </c>
+      <c r="C126" t="s">
         <v>235</v>
-      </c>
-      <c r="C126" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
+        <v>236</v>
+      </c>
+      <c r="C127" t="s">
         <v>237</v>
-      </c>
-      <c r="C127" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
+        <v>238</v>
+      </c>
+      <c r="C128" t="s">
         <v>239</v>
-      </c>
-      <c r="C128" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
+        <v>240</v>
+      </c>
+      <c r="C129" t="s">
         <v>241</v>
-      </c>
-      <c r="C129" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
+        <v>242</v>
+      </c>
+      <c r="C130" t="s">
         <v>243</v>
-      </c>
-      <c r="C130" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
+        <v>244</v>
+      </c>
+      <c r="C131" t="s">
         <v>245</v>
-      </c>
-      <c r="C131" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C132" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
+        <v>247</v>
+      </c>
+      <c r="C133" t="s">
         <v>248</v>
-      </c>
-      <c r="C133" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
+        <v>249</v>
+      </c>
+      <c r="C134" t="s">
         <v>250</v>
-      </c>
-      <c r="C134" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
+        <v>251</v>
+      </c>
+      <c r="C135" t="s">
         <v>252</v>
-      </c>
-      <c r="C135" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
+        <v>253</v>
+      </c>
+      <c r="C136" t="s">
         <v>254</v>
-      </c>
-      <c r="C136" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
+        <v>255</v>
+      </c>
+      <c r="C137" t="s">
         <v>256</v>
-      </c>
-      <c r="C137" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
+        <v>257</v>
+      </c>
+      <c r="C138" t="s">
         <v>258</v>
-      </c>
-      <c r="C138" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
+        <v>259</v>
+      </c>
+      <c r="C139" t="s">
         <v>260</v>
-      </c>
-      <c r="C139" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
+        <v>261</v>
+      </c>
+      <c r="C140" t="s">
         <v>262</v>
-      </c>
-      <c r="C140" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C141" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
+        <v>264</v>
+      </c>
+      <c r="C142" t="s">
         <v>265</v>
-      </c>
-      <c r="C142" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
+        <v>266</v>
+      </c>
+      <c r="C143" t="s">
         <v>267</v>
-      </c>
-      <c r="C143" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
+        <v>268</v>
+      </c>
+      <c r="C144" t="s">
         <v>269</v>
-      </c>
-      <c r="C144" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
+        <v>270</v>
+      </c>
+      <c r="C145" t="s">
         <v>271</v>
-      </c>
-      <c r="C145" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
+        <v>272</v>
+      </c>
+      <c r="C146" t="s">
         <v>273</v>
-      </c>
-      <c r="C146" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
+        <v>274</v>
+      </c>
+      <c r="C147" t="s">
         <v>275</v>
-      </c>
-      <c r="C147" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
+        <v>276</v>
+      </c>
+      <c r="C148" t="s">
         <v>277</v>
-      </c>
-      <c r="C148" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
+        <v>278</v>
+      </c>
+      <c r="C149" t="s">
         <v>279</v>
-      </c>
-      <c r="C149" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
+        <v>280</v>
+      </c>
+      <c r="C150" t="s">
         <v>281</v>
-      </c>
-      <c r="C150" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
+        <v>282</v>
+      </c>
+      <c r="C151" t="s">
         <v>283</v>
-      </c>
-      <c r="C151" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
+        <v>284</v>
+      </c>
+      <c r="C152" t="s">
         <v>285</v>
-      </c>
-      <c r="C152" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
+        <v>286</v>
+      </c>
+      <c r="C153" t="s">
         <v>287</v>
-      </c>
-      <c r="C153" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
+        <v>288</v>
+      </c>
+      <c r="C154" t="s">
         <v>289</v>
-      </c>
-      <c r="C154" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
+        <v>290</v>
+      </c>
+      <c r="C155" t="s">
         <v>291</v>
-      </c>
-      <c r="C155" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
+        <v>292</v>
+      </c>
+      <c r="C156" t="s">
         <v>293</v>
-      </c>
-      <c r="C156" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
+        <v>294</v>
+      </c>
+      <c r="C157" t="s">
         <v>295</v>
-      </c>
-      <c r="C157" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C158" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
+        <v>297</v>
+      </c>
+      <c r="C159" t="s">
         <v>298</v>
-      </c>
-      <c r="C159" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
+        <v>299</v>
+      </c>
+      <c r="C160" t="s">
         <v>300</v>
-      </c>
-      <c r="C160" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C161" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
+        <v>302</v>
+      </c>
+      <c r="C162" t="s">
         <v>303</v>
-      </c>
-      <c r="C162" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
+        <v>304</v>
+      </c>
+      <c r="C163" t="s">
         <v>305</v>
-      </c>
-      <c r="C163" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
+        <v>306</v>
+      </c>
+      <c r="C164" t="s">
         <v>307</v>
-      </c>
-      <c r="C164" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C165" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
+        <v>309</v>
+      </c>
+      <c r="C166" t="s">
         <v>310</v>
-      </c>
-      <c r="C166" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
+        <v>311</v>
+      </c>
+      <c r="C167" t="s">
         <v>312</v>
-      </c>
-      <c r="C167" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
+        <v>313</v>
+      </c>
+      <c r="C168" t="s">
         <v>314</v>
-      </c>
-      <c r="C168" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
+        <v>315</v>
+      </c>
+      <c r="C169" t="s">
         <v>316</v>
-      </c>
-      <c r="C169" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
+        <v>317</v>
+      </c>
+      <c r="C170" t="s">
         <v>318</v>
-      </c>
-      <c r="C170" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
+        <v>319</v>
+      </c>
+      <c r="C171" t="s">
         <v>320</v>
-      </c>
-      <c r="C171" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
+        <v>321</v>
+      </c>
+      <c r="C172" t="s">
         <v>322</v>
-      </c>
-      <c r="C172" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
+        <v>323</v>
+      </c>
+      <c r="B173" t="s">
         <v>324</v>
-      </c>
-      <c r="B173" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
+        <v>325</v>
+      </c>
+      <c r="C174" t="s">
         <v>326</v>
-      </c>
-      <c r="C174" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
+        <v>327</v>
+      </c>
+      <c r="C175" t="s">
         <v>328</v>
-      </c>
-      <c r="C175" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
+        <v>329</v>
+      </c>
+      <c r="C176" t="s">
         <v>330</v>
-      </c>
-      <c r="C176" t="s">
-        <v>331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>